<commit_message>
update dq messages and test data
</commit_message>
<xml_diff>
--- a/examples/Data/Export/Datenqualitätsreport_ dqTestData_KT .xlsx
+++ b/examples/Data/Export/Datenqualitätsreport_ dqTestData_KT .xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -388,209 +388,215 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>P_20085751</t>
+          <t>P_20085651</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>F_101645</t>
+          <t>F_101641</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>G70</t>
+          <t>E75.0</t>
         </is>
       </c>
       <c r="D2">
-        <v>586</v>
+        <v>846</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation G70 - 586 ist im BfArM nicht vorhanden. </t>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E75.0 - 846 ist im BfArM nicht vorhanden.  </t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>P_20085752</t>
+          <t>P_20085652</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>F_101646</t>
+          <t>F_101642</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>G70</t>
+          <t>E75.0</t>
         </is>
       </c>
       <c r="D3">
-        <v>589</v>
+        <v>797</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation G70 - 589 ist im BfArM nicht vorhanden. </t>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E75.0 - 797 ist im BfArM nicht vorhanden.  </t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>P_20085754</t>
+          <t>P_20085653</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>F_101648</t>
+          <t>F_101643</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>E84.80</t>
+          <t>E75.0</t>
         </is>
       </c>
       <c r="D4">
-        <v>588</v>
+        <v>309151</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E84.80 - 588 ist im BfArM nicht vorhanden.  </t>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E75.0 - 309151 ist im BfArM nicht vorhanden.  </t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>P_20085755</t>
+          <t>P_20085654</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>F_101649</t>
+          <t>F_101644</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>E75.2</t>
+          <t>E75.0</t>
         </is>
       </c>
       <c r="D5">
-        <v>325</v>
+        <v>309247</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E75.2 - 325 ist im BfArM nicht vorhanden.  </t>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E75.0 - 309247 ist im BfArM nicht vorhanden.  </t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>P_20085756</t>
+          <t>P_20085751</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>F_101650</t>
+          <t>F_101645</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>E75.2</t>
+          <t>G70.0</t>
         </is>
       </c>
       <c r="D6">
-        <v>320</v>
+        <v>586</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E75.2 - 320 ist im BfArM nicht vorhanden.  </t>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation G70.0 - 586 ist im BfArM nicht vorhanden.  </t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>P_20085757</t>
+          <t>P_20085752</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>F_101651</t>
+          <t>F_101646</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>I50.0</t>
         </is>
       </c>
       <c r="D7">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fehlendes ICD10 Code.  </t>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. ICD10 Code I50.0 ist im BfArM Mapping nicht enthalten.  </t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>P_20085758</t>
+          <t>P_20085753</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>F_101651</t>
+          <t>F_101647</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>E75.2</t>
         </is>
       </c>
       <c r="D8">
-        <v>587</v>
+        <v>3</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Orpha Kodierung 587 ist im BfArM-Mapping nicht enthalten.  Fehlendes ICD10 Code.  </t>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E75.2 - 3 ist im BfArM nicht vorhanden.  </t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>P_20085759</t>
+          <t>P_20085757</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>F_101653</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>E84.0</t>
-        </is>
+          <t>F_101651</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>586</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fehlendes Orpha_Kode.  </t>
+          <t xml:space="preserve">Fehlendes ICD10 Code.  </t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>P_20085760</t>
+          <t>P_20085758</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>F_101654</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>D45</t>
-        </is>
+          <t>F_101652</t>
+        </is>
+      </c>
+      <c r="D10">
+        <v>3</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fehlendes Orpha_Kode.  </t>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. Orpha Code 3 ist im BfArM-Mapping nicht enthalten.  Fehlendes ICD10 Code.  </t>
         </is>
       </c>
     </row>
@@ -607,7 +613,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fehlendes ICD10 Code.  </t>
+          <t xml:space="preserve">Fall ist nicht eindeutig. Fehlendes ICD10 Code.  </t>
         </is>
       </c>
     </row>
@@ -639,47 +645,207 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>P_20085764</t>
+          <t>P_20085763</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>F_101658</t>
+          <t>F_101657</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>E75.2</t>
-        </is>
+          <t>G35.9</t>
+        </is>
+      </c>
+      <c r="D13">
+        <v>71529</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICD10 Kodierung E75.2 ist nicht eindeutig. ICD10-Orpha Relation ist gemäß Tracer-Diagnosenliste vom Typ 1-m.  Fehlendes Orpha_Kode.  </t>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation G35.9 - 71529 ist im BfArM nicht vorhanden.  </t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>P_20085765</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>F_101658</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>E75.2</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ICD10 Kodierung E75.2 ist nicht eindeutig. ICD10-Orpha Relation ist gemäß Tracer-Diagnosenliste vom Typ 1-m.  Fehlendes Orpha_Kode.  </t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>P_20085766</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>F_101659</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>E75.0</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ICD10 Kodierung E75.0 ist nicht eindeutig. ICD10-Orpha Relation ist gemäß Tracer-Diagnosenliste vom Typ 1-m.  Fehlendes Orpha_Kode.  </t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>P_20085767</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>F_101660</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>E85.0</t>
-        </is>
-      </c>
-      <c r="D14">
-        <v>586</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E85.0 - 586 ist im BfArM nicht vorhanden.  </t>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>E74.0</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ICD10 Kodierung E74.0 ist nicht eindeutig. ICD10-Orpha Relation ist gemäß Tracer-Diagnosenliste vom Typ 1-m.  Fehlendes Orpha_Kode.  </t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>P_20085768</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>F_101661</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>E75.2</t>
+        </is>
+      </c>
+      <c r="D17">
+        <v>342</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E75.2 - 342 ist im BfArM nicht vorhanden.  </t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>P_20085769</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>F_101662</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>E75.0</t>
+        </is>
+      </c>
+      <c r="D18">
+        <v>226</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E75.0 - 226 ist im BfArM nicht vorhanden.  </t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>P_20085772</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>F_101665</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>D45</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fehlendes Orpha_Kode.  </t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>P_20085773</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>F_101666</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>E84.0</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fehlendes Orpha_Kode.  </t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>P_20085774</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>F_101667</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>E84.1</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fehlendes Orpha_Kode.  </t>
         </is>
       </c>
     </row>
@@ -750,28 +916,28 @@
         </is>
       </c>
       <c r="B2">
-        <v>27.68</v>
+        <v>44.29</v>
       </c>
       <c r="C2">
-        <v>72.31999999999999</v>
+        <v>55.71</v>
       </c>
       <c r="D2">
-        <v>72.73</v>
+        <v>68.42</v>
       </c>
       <c r="E2">
-        <v>60</v>
+        <v>37.5</v>
       </c>
       <c r="F2">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G2">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I2">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add DQ Indicator for outliers
</commit_message>
<xml_diff>
--- a/examples/Data/Export/Datenqualitätsreport_ dqTestData_KT .xlsx
+++ b/examples/Data/Export/Datenqualitätsreport_ dqTestData_KT .xlsx
@@ -406,7 +406,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E75.0 - 846 ist im BfArM nicht vorhanden.  </t>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E75.0 - 846 ist im BfArM nicht vorhanden.  ICD10-Orpha Zuordnung ist gemäß BfArM nicht plausible. </t>
         </is>
       </c>
     </row>
@@ -431,7 +431,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E75.0 - 797 ist im BfArM nicht vorhanden.  </t>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E75.0 - 797 ist im BfArM nicht vorhanden.  ICD10-Orpha Zuordnung ist gemäß BfArM nicht plausible. </t>
         </is>
       </c>
     </row>
@@ -456,7 +456,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E75.0 - 309151 ist im BfArM nicht vorhanden.  </t>
+          <t xml:space="preserve">Orpha Code 309151 ist im BfArM-Mapping nicht enthalten.  Kodierung ist nicht eindeutig. Relation E75.0 - 309151 ist im BfArM nicht vorhanden.  ICD10-Orpha Zuordnung ist gemäß BfArM nicht plausible. </t>
         </is>
       </c>
     </row>
@@ -481,7 +481,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E75.0 - 309247 ist im BfArM nicht vorhanden.  </t>
+          <t xml:space="preserve">Orpha Code 309247 ist im BfArM-Mapping nicht enthalten.  Kodierung ist nicht eindeutig. Relation E75.0 - 309247 ist im BfArM nicht vorhanden.  ICD10-Orpha Zuordnung ist gemäß BfArM nicht plausible. </t>
         </is>
       </c>
     </row>
@@ -498,7 +498,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>G70.0</t>
+          <t>G70</t>
         </is>
       </c>
       <c r="D6">
@@ -506,7 +506,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation G70.0 - 586 ist im BfArM nicht vorhanden.  </t>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. ICD10 Code G70 ist im BfArM Mapping nicht enthalten.  ICD10-Orpha Zuordnung ist gemäß BfArM nicht plausible. </t>
         </is>
       </c>
     </row>
@@ -523,7 +523,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>I50.0</t>
+          <t>G70</t>
         </is>
       </c>
       <c r="D7">
@@ -531,7 +531,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kodierung ist nicht eindeutig. ICD10 Code I50.0 ist im BfArM Mapping nicht enthalten.  </t>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. ICD10 Code G70 ist im BfArM Mapping nicht enthalten.  ICD10-Orpha Zuordnung ist gemäß BfArM nicht plausible. </t>
         </is>
       </c>
     </row>
@@ -548,15 +548,15 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>E75.2</t>
+          <t>E84.80</t>
         </is>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>589</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E75.2 - 3 ist im BfArM nicht vorhanden.  </t>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E84.80 - 589 ist im BfArM nicht vorhanden.  ICD10-Orpha Zuordnung ist gemäß BfArM nicht plausible. </t>
         </is>
       </c>
     </row>
@@ -596,7 +596,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kodierung ist nicht eindeutig. Orpha Code 3 ist im BfArM-Mapping nicht enthalten.  Fehlendes ICD10 Code.  </t>
+          <t xml:space="preserve">Orpha Code 3 ist im BfArM-Mapping nicht enthalten.  Fehlendes ICD10 Code.  </t>
         </is>
       </c>
     </row>
@@ -638,7 +638,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E66.89 - 320 ist im BfArM nicht vorhanden.  </t>
+          <t xml:space="preserve">Orpha Code 320 ist im BfArM-Mapping nicht enthalten.  Kodierung ist nicht eindeutig. Relation E66.89 - 320 ist im BfArM nicht vorhanden.  ICD10-Orpha Zuordnung ist gemäß BfArM nicht plausible. </t>
         </is>
       </c>
     </row>
@@ -663,7 +663,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation G35.9 - 71529 ist im BfArM nicht vorhanden.  </t>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation G35.9 - 71529 ist im BfArM nicht vorhanden.  ICD10-Orpha Zuordnung ist gemäß BfArM nicht plausible. </t>
         </is>
       </c>
     </row>
@@ -754,7 +754,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E75.2 - 342 ist im BfArM nicht vorhanden.  </t>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E75.2 - 342 ist im BfArM nicht vorhanden.  ICD10-Orpha Zuordnung ist gemäß BfArM nicht plausible. </t>
         </is>
       </c>
     </row>
@@ -779,7 +779,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E75.0 - 226 ist im BfArM nicht vorhanden.  </t>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E75.0 - 226 ist im BfArM nicht vorhanden.  ICD10-Orpha Zuordnung ist gemäß BfArM nicht plausible. </t>
         </is>
       </c>
     </row>
@@ -856,7 +856,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -875,7 +875,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>completness_rate</t>
+          <t>outlier_rate</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -890,20 +890,30 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>icdRd_no</t>
+          <t>orphaCoding_plausibility_rate</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>rd_no</t>
+          <t>orphaCoding_relativeFrequency</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>orphaCoding_absoluteFrequency</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>uniqueRd_no</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>pt_no</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>case_no</t>
         </is>
@@ -916,27 +926,33 @@
         </is>
       </c>
       <c r="B2">
-        <v>44.29</v>
+        <v>40.82</v>
       </c>
       <c r="C2">
-        <v>55.71</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>68.42</v>
+        <v>66.67</v>
       </c>
       <c r="E2">
         <v>37.5</v>
       </c>
       <c r="F2">
-        <v>19</v>
+        <v>31.25</v>
       </c>
       <c r="G2">
+        <v>1.4</v>
+      </c>
+      <c r="H2">
+        <v>14</v>
+      </c>
+      <c r="I2">
         <v>9</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>27</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>28</v>
       </c>
     </row>

</xml_diff>